<commit_message>
issue 246 && 267 && 248
</commit_message>
<xml_diff>
--- a/public/template/o_import.xlsx
+++ b/public/template/o_import.xlsx
@@ -4,11 +4,27 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12540"/>
+    <workbookView windowWidth="28800" windowHeight="12540" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="硬件整机测试字段" sheetId="9" r:id="rId1"/>
+    <sheet name="整机数据" sheetId="9" r:id="rId1"/>
+    <sheet name="整机分类" sheetId="10" r:id="rId2"/>
+    <sheet name="适配状态" sheetId="11" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="待验证">适配状态!$D$2:$D$2</definedName>
+    <definedName name="适配暂停">适配状态!$E$2:$E$4</definedName>
+    <definedName name="适配中">适配状态!$B$2:$B$18</definedName>
+    <definedName name="未适配">适配状态!$A$2:$A$4</definedName>
+    <definedName name="已适配">适配状态!$C$2:$C$12</definedName>
+    <definedName name="其它">整机分类!$G$2:$G$2</definedName>
+    <definedName name="处理器">整机分类!$A$2:$A$3</definedName>
+    <definedName name="板卡">整机分类!$B$2:$B$14</definedName>
+    <definedName name="存储">整机分类!$C$2:$C$10</definedName>
+    <definedName name="服务器">整机分类!$D$2:$D$3</definedName>
+    <definedName name="桌面终端">整机分类!$E$2:$E$5</definedName>
+    <definedName name="工作站">整机分类!$F$2:$F$2</definedName>
+  </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
@@ -70,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="125">
   <si>
     <t>厂商</t>
   </si>
@@ -192,6 +208,12 @@
     <t>备注</t>
   </si>
   <si>
+    <t>处理器</t>
+  </si>
+  <si>
+    <t>CPU</t>
+  </si>
+  <si>
     <t>厂商主动申请</t>
   </si>
   <si>
@@ -204,6 +226,12 @@
     <t>arm64</t>
   </si>
   <si>
+    <t>未适配</t>
+  </si>
+  <si>
+    <t>厂商暂无适配计划</t>
+  </si>
+  <si>
     <t>CERTIFICATION</t>
   </si>
   <si>
@@ -211,6 +239,228 @@
   </si>
   <si>
     <t>是</t>
+  </si>
+  <si>
+    <t>板卡</t>
+  </si>
+  <si>
+    <t>存储</t>
+  </si>
+  <si>
+    <t>服务器</t>
+  </si>
+  <si>
+    <t>桌面终端</t>
+  </si>
+  <si>
+    <t>工作站</t>
+  </si>
+  <si>
+    <t>其它</t>
+  </si>
+  <si>
+    <t>内存</t>
+  </si>
+  <si>
+    <t>磁盘</t>
+  </si>
+  <si>
+    <t>服务器整机</t>
+  </si>
+  <si>
+    <t>PC整机</t>
+  </si>
+  <si>
+    <t>其他</t>
+  </si>
+  <si>
+    <t>GPU</t>
+  </si>
+  <si>
+    <t>声卡</t>
+  </si>
+  <si>
+    <t>移动存储</t>
+  </si>
+  <si>
+    <t>堡垒机</t>
+  </si>
+  <si>
+    <t>笔记本</t>
+  </si>
+  <si>
+    <t>显卡</t>
+  </si>
+  <si>
+    <t>存储阵列</t>
+  </si>
+  <si>
+    <t>工控机</t>
+  </si>
+  <si>
+    <t>RAID卡</t>
+  </si>
+  <si>
+    <t>网络存储</t>
+  </si>
+  <si>
+    <t>云终端</t>
+  </si>
+  <si>
+    <t>AI加速卡</t>
+  </si>
+  <si>
+    <t>负载均衡器</t>
+  </si>
+  <si>
+    <t>PXIe</t>
+  </si>
+  <si>
+    <t>统一存储</t>
+  </si>
+  <si>
+    <t>RTC</t>
+  </si>
+  <si>
+    <t>分布式存储</t>
+  </si>
+  <si>
+    <t>HBA</t>
+  </si>
+  <si>
+    <t>对象存储</t>
+  </si>
+  <si>
+    <t>HCA</t>
+  </si>
+  <si>
+    <t>光盘存储</t>
+  </si>
+  <si>
+    <t>加解密卡</t>
+  </si>
+  <si>
+    <t>主板</t>
+  </si>
+  <si>
+    <t>串口卡</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>适配中</t>
+  </si>
+  <si>
+    <t>已适配</t>
+  </si>
+  <si>
+    <t>待验证</t>
+  </si>
+  <si>
+    <t>适配暂停</t>
+  </si>
+  <si>
+    <t>云平台资源准备中</t>
+  </si>
+  <si>
+    <t>互认证证书制作中</t>
+  </si>
+  <si>
+    <t>麒麟自研适配方案，待内部验证</t>
+  </si>
+  <si>
+    <t>麒麟原因</t>
+  </si>
+  <si>
+    <t>待与厂商沟通</t>
+  </si>
+  <si>
+    <t>适配方案开发中</t>
+  </si>
+  <si>
+    <t>证书邮寄中（后期）</t>
+  </si>
+  <si>
+    <t>厂商原因</t>
+  </si>
+  <si>
+    <t>与厂商正在沟通</t>
+  </si>
+  <si>
+    <t>厂商安排测试环境中</t>
+  </si>
+  <si>
+    <t>证书归档中（后期）</t>
+  </si>
+  <si>
+    <t>其他原因</t>
+  </si>
+  <si>
+    <t>测试相关设备借收货中</t>
+  </si>
+  <si>
+    <t>证书已归档</t>
+  </si>
+  <si>
+    <t>厂商适配申请准备中</t>
+  </si>
+  <si>
+    <t>测试报告已上传至生态网站</t>
+  </si>
+  <si>
+    <t>适配申请生态审核中</t>
+  </si>
+  <si>
+    <t>适配成果数据已更新至生态网站</t>
+  </si>
+  <si>
+    <t>适配测试中—远程测试</t>
+  </si>
+  <si>
+    <t>适配成果已上架至软件商店</t>
+  </si>
+  <si>
+    <t>适配测试中—出差测试</t>
+  </si>
+  <si>
+    <t>麒麟自研适配方案，内部已验证通过</t>
+  </si>
+  <si>
+    <t>适配测试中—视频复测</t>
+  </si>
+  <si>
+    <t>适配成果已提交上架软件商店</t>
+  </si>
+  <si>
+    <t>适配测试中—麒麟内测</t>
+  </si>
+  <si>
+    <t>排期待适配测试</t>
+  </si>
+  <si>
+    <t>适配问题定位分析中</t>
+  </si>
+  <si>
+    <t>适配成果已下架软件商店</t>
+  </si>
+  <si>
+    <t>问题修复中—厂商问题</t>
+  </si>
+  <si>
+    <t>问题修复中—系统问题</t>
+  </si>
+  <si>
+    <t>问题修复中—其他问题</t>
+  </si>
+  <si>
+    <t>问题复测中</t>
+  </si>
+  <si>
+    <t>测试报告确认中</t>
+  </si>
+  <si>
+    <t>适配成果已提交下架软件商店</t>
   </si>
 </sst>
 </file>
@@ -218,14 +468,27 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="31">
     <font>
       <sz val="11"/>
+      <name val="等线"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="等线"/>
       <charset val="134"/>
     </font>
@@ -266,6 +529,50 @@
       <sz val="10"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -276,18 +583,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="宋体"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -299,15 +606,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -321,13 +638,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -336,76 +646,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -419,9 +661,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -429,6 +680,11 @@
       <name val="宋体"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -439,181 +695,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -661,15 +917,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -685,17 +932,35 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -715,26 +980,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -763,192 +1019,198 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="11" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="49" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="49" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1273,8 +1535,8 @@
   <sheetPr/>
   <dimension ref="A1:AN2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1"/>
@@ -1282,220 +1544,636 @@
     <col min="5" max="5" width="13.375" customWidth="1"/>
     <col min="15" max="16" width="16.375" customWidth="1"/>
     <col min="18" max="18" width="9.50833333333333" customWidth="1"/>
-    <col min="25" max="27" width="9" style="1"/>
-    <col min="28" max="28" width="13.125" style="1" customWidth="1"/>
-    <col min="29" max="40" width="9" style="1"/>
+    <col min="25" max="27" width="9" style="4"/>
+    <col min="28" max="28" width="13.125" style="4" customWidth="1"/>
+    <col min="29" max="40" width="9" style="4"/>
   </cols>
   <sheetData>
     <row r="1" ht="54" customHeight="1" spans="1:40">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="O1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="P1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="R1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="S1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="T1" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="U1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="W1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="X1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="9" t="s">
+      <c r="Y1" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="9" t="s">
+      <c r="Z1" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="9" t="s">
+      <c r="AA1" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="9" t="s">
+      <c r="AB1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="9" t="s">
+      <c r="AC1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="9" t="s">
+      <c r="AD1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="9" t="s">
+      <c r="AE1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AF1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AG1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AH1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AI1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AJ1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AK1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="9" t="s">
+      <c r="AL1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="9" t="s">
+      <c r="AM1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="12" t="s">
+      <c r="AN1" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1" spans="1:40">
-      <c r="A2" s="4"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="8" t="s">
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6" t="s">
+      <c r="I2" s="9"/>
+      <c r="J2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6" t="s">
+      <c r="K2" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="L2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="S2" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="T2" s="6"/>
-      <c r="U2" s="6"/>
-      <c r="V2" s="6"/>
-      <c r="W2" s="6"/>
-      <c r="X2" s="6"/>
-      <c r="Y2" s="10"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11"/>
-      <c r="AM2" s="11"/>
-      <c r="AN2" s="11"/>
+      <c r="M2" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="T2" s="9"/>
+      <c r="U2" s="9"/>
+      <c r="V2" s="9"/>
+      <c r="W2" s="9"/>
+      <c r="X2" s="9"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="13"/>
+      <c r="AA2" s="13"/>
+      <c r="AB2" s="13"/>
+      <c r="AC2" s="13"/>
+      <c r="AD2" s="13"/>
+      <c r="AE2" s="13"/>
+      <c r="AF2" s="13"/>
+      <c r="AG2" s="13"/>
+      <c r="AH2" s="13"/>
+      <c r="AI2" s="13"/>
+      <c r="AJ2" s="13"/>
+      <c r="AK2" s="13"/>
+      <c r="AL2" s="13"/>
+      <c r="AM2" s="13"/>
+      <c r="AN2" s="13"/>
     </row>
   </sheetData>
-  <dataValidations count="8">
+  <dataValidations count="10">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
+      <formula1>"arm64,amd64,mips64el,loongarch64,sw64"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
+      <formula1>"飞腾,鲲鹏,兆芯,海光,龙芯MIPS,龙芯LoongArch,申威,AMD,Intel,海思麒麟990,海思麒麟9006c,盘古M900"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2 M2">
+      <formula1>INDIRECT(OFFSET(INDIRECT(ADDRESS(ROW(),COLUMN())),0,-1))</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2">
-      <formula1>"厂商主动申请,BD主动拓展,行业营销中心引入,区域营销中心引入,最终客户反馈,产品经理引入,厂商合作事业本部引入,渠道部引入,相关机构反馈,其他方式引入"</formula1>
+      <formula1>整机分类!$A$1:$E$1</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
+      <formula1>"银河麒麟桌面操作系统V10SP1,银河麒麟桌面操作系统V10,银河麒麟桌面操作系统V4,中标麒麟桌面操作系统V7,银河麒麟服务器操作系统V10SP1,银河麒麟服务器操作系统V10,银河麒麟服务器操作系统V4,中标麒麟服务器操作系统V7,银河麒麟服务器操作系统V10SP2,银河麒麟桌面操作系统（金融机具版）V10,银河麒麟桌面操作系统（工控机版）V10,银河麒麟桌面操作系统（教育版）V10,银河麒麟桌面操作系统（大屏版）V10SP1"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2 S2 T2 U2">
+      <formula1>"是,否"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L2">
       <formula1>"未适配,适配中,已适配,待验证,适配暂停"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2">
-      <formula1>"银河麒麟桌面操作系统V10SP1,银河麒麟桌面操作系统V10,银河麒麟桌面操作系统V4,中标麒麟桌面操作系统V7,银河麒麟服务器操作系统V10SP1,银河麒麟服务器操作系统V10,银河麒麟服务器操作系统V4,中标麒麟服务器操作系统V7,银河麒麟服务器操作系统V10SP2,银河麒麟桌面操作系统（金融机具版）V10,银河麒麟桌面操作系统（工控机版）V10,银河麒麟桌面操作系统（教育版）V10,银河麒麟桌面操作系统（大屏版）V10SP1"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2 P2">
+      <formula1>"READY,CERTIFICATION,VALIDATION"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="Q2">
       <formula1>"厂商自测,测试部测试,区域适配中心测试,第三方测试,技服FAE测试"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2">
-      <formula1>"飞腾,鲲鹏,兆芯,海光,龙芯MIPS,龙芯LoongArch,申威,AMD,Intel,海思麒麟990,海思麒麟9006c,盘古M900"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2">
-      <formula1>"arm64,amd64,mips64el,loongarch64,sw64"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="O2 P2">
-      <formula1>"READY,CERTIFICATION,VALIDATION"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R2 S2 T2 U2">
-      <formula1>"是,否"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C30">
+      <formula1>整机分类!$A$1:$G$1</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5">
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" t="s">
+        <v>68</v>
+      </c>
+      <c r="E4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5">
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C5" t="s">
+        <v>71</v>
+      </c>
+      <c r="E5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3">
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3">
+      <c r="B7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3">
+      <c r="B8" t="s">
+        <v>77</v>
+      </c>
+      <c r="C8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3">
+      <c r="B9" t="s">
+        <v>79</v>
+      </c>
+      <c r="C9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3">
+      <c r="B10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>86</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection password="F6EA" sheet="1" objects="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="17.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="21.375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="33.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="29.625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1"/>
+    <col min="6" max="16384" width="9" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="14.25" spans="1:5">
+      <c r="A1" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="2" ht="14.25" spans="1:5">
+      <c r="A2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="3" ht="14.25" spans="1:5">
+      <c r="A3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" ht="14.25" spans="1:5">
+      <c r="A4" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" ht="14.25" spans="1:5">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" ht="14.25" spans="1:5">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" ht="14.25" spans="1:5">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" ht="14.25" spans="1:5">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="3"/>
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" ht="14.25" spans="1:5">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" ht="14.25" spans="1:5">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" ht="14.25" spans="1:5">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" ht="14.25" spans="1:5">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" ht="14.25" spans="1:5">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" ht="14.25" spans="1:5">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" ht="14.25" spans="1:5">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" ht="14.25" spans="1:5">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" ht="14.25" spans="1:5">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" ht="14.25" spans="1:5">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" ht="14.25" spans="1:5">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+    </row>
+  </sheetData>
+  <sheetProtection password="F6EA" sheet="1" objects="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>